<commit_message>
update header on all pendampingan files template
</commit_message>
<xml_diff>
--- a/frontend/public/example_pendampingan_anak.xlsx
+++ b/frontend/public/example_pendampingan_anak.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSI\Documents\khoir\freelance\test\pops_apps\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5EDC8C-ECC3-4B97-927C-3575DCBC8362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC09CAA8-9543-41CC-BE63-1573A785E742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="420" windowWidth="17280" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BALITA_TPK (1)" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>KECAMATAN</t>
   </si>
   <si>
-    <t>Desa di Kec. Bulakamba</t>
-  </si>
-  <si>
     <t>RT</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>`1871000000000030</t>
+  </si>
+  <si>
+    <t>Desa</t>
   </si>
 </sst>
 </file>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AK5" sqref="AK5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -595,79 +595,79 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:45">
@@ -675,43 +675,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
       </c>
       <c r="G2">
         <v>49</v>
       </c>
       <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" t="s">
-        <v>61</v>
-      </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2">
         <v>39</v>
       </c>
       <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
         <v>48</v>
-      </c>
-      <c r="M2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" t="s">
-        <v>49</v>
       </c>
       <c r="O2">
         <v>43</v>
@@ -720,19 +720,19 @@
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" t="s">
         <v>51</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>52</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>53</v>
-      </c>
-      <c r="U2" t="s">
-        <v>54</v>
       </c>
       <c r="V2">
         <v>1</v>
@@ -753,7 +753,7 @@
         <v>103.7</v>
       </c>
       <c r="AB2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AC2">
         <v>15</v>
@@ -762,40 +762,40 @@
         <v>50</v>
       </c>
       <c r="AE2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AF2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="AM2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP2" t="s">
         <v>57</v>
       </c>
-      <c r="AM2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>58</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AR2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AS2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save cadre, keluarga, and anggota keluarga
</commit_message>
<xml_diff>
--- a/frontend/public/example_pendampingan_anak.xlsx
+++ b/frontend/public/example_pendampingan_anak.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSI\Documents\khoir\freelance\test\pops_apps\frontend\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC09CAA8-9543-41CC-BE63-1573A785E742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="420" windowWidth="17280" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="BALITA_TPK (1)" sheetId="1" r:id="rId1"/>
@@ -82,6 +76,9 @@
     <t>KECAMATAN</t>
   </si>
   <si>
+    <t>Desa</t>
+  </si>
+  <si>
     <t>RT</t>
   </si>
   <si>
@@ -151,21 +148,33 @@
     <t>Ratna dewi</t>
   </si>
   <si>
-    <t>24/12/25</t>
+    <t>24/12/2025</t>
   </si>
   <si>
     <t>WIJAYA SAPUTRA</t>
   </si>
   <si>
+    <t>`1871000000000033</t>
+  </si>
+  <si>
     <t>LAKI-LAKI</t>
   </si>
   <si>
+    <t>DASLAM</t>
+  </si>
+  <si>
+    <t>`1871000000000001</t>
+  </si>
+  <si>
     <t>Dagang</t>
   </si>
   <si>
     <t>Solikhah</t>
   </si>
   <si>
+    <t>`1871000000000030</t>
+  </si>
+  <si>
     <t>Wiraswasta</t>
   </si>
   <si>
@@ -194,28 +203,19 @@
   </si>
   <si>
     <t>Dirujuk</t>
-  </si>
-  <si>
-    <t>`1871000000000033</t>
-  </si>
-  <si>
-    <t>DASLAM</t>
-  </si>
-  <si>
-    <t>`1871000000000001</t>
-  </si>
-  <si>
-    <t>`1871000000000030</t>
-  </si>
-  <si>
-    <t>Desa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,16 +223,346 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -240,9 +570,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -251,17 +823,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -519,19 +1135,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:45">
       <c r="A1" t="s">
@@ -595,79 +1211,79 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AG1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AH1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AJ1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AK1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AL1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AM1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AN1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AO1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AP1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AQ1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AR1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AS1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:45">
@@ -675,43 +1291,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G2">
         <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K2">
         <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="N2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O2">
         <v>43</v>
@@ -720,19 +1336,19 @@
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="R2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="S2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="T2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="U2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="V2">
         <v>1</v>
@@ -753,7 +1369,7 @@
         <v>103.7</v>
       </c>
       <c r="AB2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AC2">
         <v>15</v>
@@ -762,43 +1378,44 @@
         <v>50</v>
       </c>
       <c r="AE2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AF2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AG2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" t="s">
         <v>55</v>
       </c>
-      <c r="AH2" t="s">
-        <v>50</v>
-      </c>
       <c r="AI2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="AM2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AN2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AO2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AP2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="AQ2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AR2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AS2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>